<commit_message>
do multivariate case Pt.3
</commit_message>
<xml_diff>
--- a/examples/excel_formulas.xlsx
+++ b/examples/excel_formulas.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t/Documents/Python_Packages/techtonique-apis/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C752F3-C5D8-4C47-AA99-7927D46D9035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D9ADDC-DE17-C94E-802A-EA71472F2942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14720" xr2:uid="{866FC63A-F4EA-0B48-8E6B-E2860E222B05}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14720" activeTab="1" xr2:uid="{866FC63A-F4EA-0B48-8E6B-E2860E222B05}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="univariate" sheetId="1" r:id="rId1"/>
+    <sheet name="multivariate" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>date</t>
   </si>
@@ -277,6 +278,12 @@
   </si>
   <si>
     <t>9240.0</t>
+  </si>
+  <si>
+    <t>heater</t>
+  </si>
+  <si>
+    <t>icecream</t>
   </si>
 </sst>
 </file>
@@ -665,7 +672,7 @@
     <we:reference id="wa200008175" version="1.0.0.0" store="en-US" storeType="OMEX"/>
   </we:alternateReferences>
   <we:properties>
-    <we:property name="main.py" value="&quot;\&quot;\&quot;\&quot;\nxlwings Lite allows you to define\nautomation scripts and custom functions\nwith Python instead of VBA\/Office Scripts.\n\nSelect a function in the green dropdown\nabove and run it by clicking the button or\nor by pressing F5. One of the sample\nscripts will insert custom functions,\nwhich are defined using the @func\ndecorator. You can add, delete, or edit\nfunctions in this file.\&quot;\&quot;\&quot;\nimport tempfile\nimport datetime as dt\nimport numpy as np\nimport pandas as pd\nimport seaborn as sns\nfrom xlwings import func, arg, ret\nfrom techtonique_apis import TechtoniqueAPI\n\n@func\ndef hello(name: str):\n    # This is the easiest custom function\n    return f\&quot;Hello {name}!\&quot;\n\n\n@func\ndef standard_normal(rows, cols):\n    # Returns an array of standard normally distributed pseudo random numbers\n    rng = np.random.default_rng()\n    matrix = rng.standard_normal(size=(rows, cols))\n    date_rng = pd.date_range(start=dt.datetime(2025, 6, 15), periods=rows, freq=\&quot;D\&quot;)\n    df = pd.DataFrame(\n        matrix, columns=[f\&quot;col{i + 1}\&quot; for i in range(matrix.shape[1])], index=date_rng\n    )\n    return df\n\n\n@func\ndef correl2(df: pd.DataFrame):\n    # Like CORREL, but it works on whole matrices instead of just 2 arrays.\n    # The type hint converts the values of the range into a pandas DataFrame.\n    # Use this function on the output of the standard_normal function from above.\n    return df.corr()\n\napi = TechtoniqueAPI()\n\n@func\n@arg(\&quot;df\&quot;, index=False)\n@ret(index=False)\ndef techto_forecast(\n    df: pd.DataFrame,\n    base_model: str = \&quot;RidgeCV\&quot;,\n    n_hidden_features: int = 5,\n    lags: int = 25,\n    type_pi: str = \&quot;kde\&quot;,\n    replications: int = 10,\n    h: int = 5,\n    return_sims: bool = False \n) -&gt; pd.DataFrame:\n    \&quot;\&quot;\&quot;Forecasting: pass a time series as a DataFrame from Excel, return forecast.\&quot;\&quot;\&quot;\n    with tempfile.NamedTemporaryFile(suffix=\&quot;.csv\&quot;, delete=False) as tmp:\n        print(df.head())\n        print(df.tail())\n        df.to_csv(tmp.name, index=False)\n        result = api.forecasting(\n            file_path=tmp.name,\n            base_model=base_model,\n            n_hidden_features=n_hidden_features,\n            lags=lags,\n            type_pi=type_pi,\n            replications=replications,\n            h=h,\n        )\n    output_dates = result[\&quot;date\&quot;]\n    res_df = pd.DataFrame(result.pop('sims'))\n    if return_sims:\n        res2_df = pd.DataFrame([])\n        res2_df[\&quot;date\&quot;] = output_dates\n        sims_df = res_df.transpose()\n        sims_df.columns = [(i + 1) for i in range(sims_df.shape[1])]\n        return pd.concat([res2_df, sims_df], axis=1)\n    return pd.DataFrame(result)\n\n&quot;"/>
+    <we:property name="main.py" value="&quot;\&quot;\&quot;\&quot;\nxlwings Lite allows you to define\nautomation scripts and custom functions\nwith Python instead of VBA\/Office Scripts.\n\nSelect a function in the green dropdown\nabove and run it by clicking the button or\nor by pressing F5. One of the sample\nscripts will insert custom functions,\nwhich are defined using the @func\ndecorator. You can add, delete, or edit\nfunctions in this file.\&quot;\&quot;\&quot;\nimport tempfile\nimport datetime as dt\nimport numpy as np\nimport pandas as pd\nimport seaborn as sns\nfrom xlwings import func, arg, ret\nfrom techtonique_apis import TechtoniqueAPI\n\n@func\ndef hello(name: str):\n    # This is the easiest custom function\n    return f\&quot;Hello {name}!\&quot;\n\n\n@func\ndef standard_normal(rows, cols):\n    # Returns an array of standard normally distributed pseudo random numbers\n    rng = np.random.default_rng()\n    matrix = rng.standard_normal(size=(rows, cols))\n    date_rng = pd.date_range(start=dt.datetime(2025, 6, 15), periods=rows, freq=\&quot;D\&quot;)\n    df = pd.DataFrame(\n        matrix, columns=[f\&quot;col{i + 1}\&quot; for i in range(matrix.shape[1])], index=date_rng\n    )\n    return df\n\n\n@func\ndef correl2(df: pd.DataFrame):\n    # Like CORREL, but it works on whole matrices instead of just 2 arrays.\n    # The type hint converts the values of the range into a pandas DataFrame.\n    # Use this function on the output of the standard_normal function from above.\n    return df.corr()\n\napi = TechtoniqueAPI()\n\ndef excel_date_to_datetime(excel_serial):\n    # Excel's day 0 is 1899-12-30\n    return pd.to_datetime('1899-12-30') + pd.to_timedelta(excel_serial, unit='D')\n\n@func\n@arg(\&quot;df\&quot;, index=False)\n@ret(index=False)\ndef techto_forecast(\n    df: pd.DataFrame,\n    base_model: str = \&quot;RidgeCV\&quot;,\n    n_hidden_features: int = 5,\n    lags: int = 25,\n    type_pi: str = \&quot;kde\&quot;,\n    replications: int = 10,\n    h: int = 5,\n    return_sims: bool = False, \n    series_choice: str = None\n) -&gt; pd.DataFrame:\n    \&quot;\&quot;\&quot;Forecasting: pass a time series as a DataFrame from Excel, return forecast.\n    \n    Excel\/xlwings custom function: Forecast a time series passed as a DataFrame from Excel, using the Techtonique API.\n\n    Parameters\n    ----------\n\n    df : pd.DataFrame\n        The input time series data as a DataFrame (from Excel range).\n\n    base_model : str, default \&quot;RidgeCV\&quot;\n        The base model to use for forecasting.\n\n    n_hidden_features : int, default 5\n        Number of hidden features for the model.\n\n    lags : int, default 25\n        Number of lags to use in the model.\n\n    type_pi : str, default \&quot;kde\&quot;\n        Type of prediction interval (\&quot;kde\&quot; or other supported types).\n\n    replications : int, default 10\n        Number of simulation replications.\n\n    h : int, default 5\n        Forecast horizon (number of periods ahead to forecast).\n\n    return_sims : bool, default False\n        If True, return the simulation matrix; otherwise, return the forecast summary bounds.\n    \n    series_choice : str, optional\n        If provided, specifies which series to forecast from the DataFrame.\n\n    Returns\n    -------\n\n    pd.DataFrame\n        The forecast results or simulation matrix as a DataFrame for Excel.\n\n    \&quot;\&quot;\&quot;\n    # Convert Excel serial dates to datetime if needed\n    if pd.api.types.is_numeric_dtype(df['date']):\n        df['date'] = df['date'].apply(excel_date_to_datetime)\n\n    with tempfile.NamedTemporaryFile(suffix=\&quot;.csv\&quot;, delete=False) as tmp:\n        df.to_csv(tmp.name, index=False)\n        result = api.forecasting(\n            file_path=tmp.name,\n            base_model=base_model,\n            n_hidden_features=n_hidden_features,\n            lags=lags,\n            type_pi=type_pi,\n            replications=replications,\n            h=h,\n        )\n    output_dates = result[\&quot;date\&quot;]\n    if df.shape[1] == 2: # univariate time series\n        res_df = pd.DataFrame(result.pop('sims'))\n        if return_sims:\n            res2_df = pd.DataFrame([])\n            res2_df[\&quot;date\&quot;] = output_dates\n            sims_df = res_df.transpose()\n            sims_df.columns = [(i + 1) for i in range(sims_df.shape[1])]\n            return pd.concat([res2_df, sims_df], axis=1)\n        return pd.DataFrame(result)\n    else:  # multivariate time series\n        n_series = len(result[\&quot;mean\&quot;][0])\n        series_names = [col for col in df.columns if col != \&quot;date\&quot;]\n        if len(series_names) != n_series:\n            series_names = [f\&quot;series_{i+1}\&quot; for i in range(n_series)]\n\n        # If series_choice is provided and valid, extract its index and return as univariate\n        if series_choice is not None and series_choice in series_names:\n            idx = series_names.index(series_choice)\n            # Extract only the selected series from each stat\n            summary_df = pd.DataFrame({\n                \&quot;date\&quot;: output_dates,\n                \&quot;mean\&quot;: [x[idx] for x in result[\&quot;mean\&quot;]],\n                \&quot;lower\&quot;: [x[idx] for x in result[\&quot;lower\&quot;]],\n                \&quot;upper\&quot;: [x[idx] for x in result[\&quot;upper\&quot;]],\n            })\n            if return_sims:\n                # sims: shape (replications, horizon, n_series)\n                sims = result[\&quot;sims\&quot;]  # list of replications, each is list of horizon, each is list of n_series\n                # For each replication, extract the selected series only\n                sims_selected = [[h[idx] for h in rep] for rep in sims]  # shape: (replications, horizon)\n                sims_df = pd.DataFrame(sims_selected).transpose()\n                sims_df.columns = [f\&quot;sim_{i+1}_{series_choice}\&quot; for i in range(sims_df.shape[1])]\n                res2_df = pd.DataFrame({\&quot;date\&quot;: output_dates})\n                return pd.concat([res2_df, sims_df], axis=1)\n            return summary_df\n\n        # Otherwise, return the full multivariate summary as before\n        summary_data = {\&quot;date\&quot;: output_dates}\n        for stat in [\&quot;mean\&quot;, \&quot;lower\&quot;, \&quot;upper\&quot;]:\n            for s in range(n_series):\n                summary_data[f\&quot;{stat}_{series_names[s]}\&quot;] = [x[s] for x in result[stat]]\n        summary_df = pd.DataFrame(summary_data)\n        if return_sims:\n            # sims: shape (replications, horizon, n_series)\n            sims = result[\&quot;sims\&quot;]\n            flat = []\n            for rep in sims:\n                for s in range(n_series):\n                    flat.append([h[s] for h in rep])\n            sims_df = pd.DataFrame(flat).transpose()\n            colnames = []\n            for r in range(len(sims)):\n                for s in range(n_series):\n                    colnames.append(f\&quot;sim_{r+1}_{series_names[s]}\&quot;)\n            sims_df.columns = colnames\n            sims_df.insert(0, \&quot;date\&quot;, output_dates)\n            return sims_df\n        return summary_df\n\n\n\n&quot;"/>
     <we:property name="pyodideVersion" value="&quot;0.27.5&quot;"/>
     <we:property name="addinVersion" value="&quot;1.0.0.0-17&quot;"/>
     <we:property name="requirements.txt" value="&quot;# Pin the version of packages that are installed from PyPI.\n# Don't pin the version if they are on this list:\n# https:\/\/pyodide.org\/en\/stable\/usage\/packages-in-pyodide.html\n#\n# New packages are installed on the fly.\n# However, the following situations require a restart:\n# - removing a package\n# - changing the version of a package\n# - adding an optional dependency of xlwings, e.g, polars\n\nxlwings==0.33.14  # required\npython-dotenv==1.1.0  # required\npyodide-http  # required\nblack  # required\npandas\nmatplotlib\nseaborn\ntechtonique_apis&quot;"/>
@@ -692,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57027A3D-DA17-9D4E-A60B-0E0D8F0061BD}">
   <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="str">
-        <v>1970-01-02</v>
+        <v>1979-01-01</v>
       </c>
       <c r="E3">
         <v>7906.8902034994926</v>
@@ -755,7 +762,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="str">
-        <v>1970-01-03</v>
+        <v>1979-02-01</v>
       </c>
       <c r="E4">
         <v>7583.8343529130243</v>
@@ -775,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="str">
-        <v>1970-01-04</v>
+        <v>1979-03-01</v>
       </c>
       <c r="E5">
         <v>7988.4844280539792</v>
@@ -795,7 +802,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="str">
-        <v>1970-01-05</v>
+        <v>1979-04-01</v>
       </c>
       <c r="E6">
         <v>7818.9874263521006</v>
@@ -815,7 +822,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="str">
-        <v>1970-01-06</v>
+        <v>1979-05-01</v>
       </c>
       <c r="E7">
         <v>9102.8831435362554</v>
@@ -835,7 +842,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="str">
-        <v>1970-01-07</v>
+        <v>1979-06-01</v>
       </c>
       <c r="E8">
         <v>9240.1351442372397</v>
@@ -935,7 +942,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="str">
-        <v>1970-01-02</v>
+        <v>1979-01-01</v>
       </c>
       <c r="E11">
         <v>7433.5974876876699</v>
@@ -1006,7 +1013,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="str">
-        <v>1970-01-03</v>
+        <v>1979-02-01</v>
       </c>
       <c r="E12">
         <v>7603.3597642037239</v>
@@ -1077,7 +1084,7 @@
         <v>13</v>
       </c>
       <c r="D13" t="str">
-        <v>1970-01-04</v>
+        <v>1979-03-01</v>
       </c>
       <c r="E13">
         <v>7887.6761438309341</v>
@@ -1148,7 +1155,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="str">
-        <v>1970-01-05</v>
+        <v>1979-04-01</v>
       </c>
       <c r="E14">
         <v>7588.3995915111482</v>
@@ -1219,7 +1226,7 @@
         <v>15</v>
       </c>
       <c r="D15" t="str">
-        <v>1970-01-06</v>
+        <v>1979-05-01</v>
       </c>
       <c r="E15">
         <v>8841.5442809761935</v>
@@ -1290,7 +1297,7 @@
         <v>16</v>
       </c>
       <c r="D16" t="str">
-        <v>1970-01-07</v>
+        <v>1979-06-01</v>
       </c>
       <c r="E16">
         <v>8777.7168159683497</v>
@@ -1361,7 +1368,7 @@
         <v>17</v>
       </c>
       <c r="D17" t="str">
-        <v>1970-01-08</v>
+        <v>1979-07-01</v>
       </c>
       <c r="E17">
         <v>10313.046329828709</v>
@@ -1432,7 +1439,7 @@
         <v>18</v>
       </c>
       <c r="D18" t="str">
-        <v>1970-01-09</v>
+        <v>1979-08-01</v>
       </c>
       <c r="E18">
         <v>9875.6721995083608</v>
@@ -1503,7 +1510,7 @@
         <v>19</v>
       </c>
       <c r="D19" t="str">
-        <v>1970-01-10</v>
+        <v>1979-09-01</v>
       </c>
       <c r="E19">
         <v>8751.9042266836877</v>
@@ -1574,7 +1581,7 @@
         <v>20</v>
       </c>
       <c r="D20" t="str">
-        <v>1970-01-11</v>
+        <v>1979-10-01</v>
       </c>
       <c r="E20">
         <v>8944.5027335236846</v>
@@ -2059,6 +2066,2851 @@
       </c>
       <c r="B73" t="s">
         <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0DF073-385F-1248-B9C4-6F72C369E2B0}">
+  <dimension ref="A1:O199"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>37987</v>
+      </c>
+      <c r="B2">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="E2" t="str" cm="1">
+        <f t="array" ref="E2:H8">_xldudf_TECHTO_FORECAST($A$1:$C$199,"Ridge",5,20,,,6,FALSE,"icecream")</f>
+        <v>date</v>
+      </c>
+      <c r="F2" t="str">
+        <v>mean</v>
+      </c>
+      <c r="G2" t="str">
+        <v>lower</v>
+      </c>
+      <c r="H2" t="str">
+        <v>upper</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>38018</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="E3" t="str">
+        <v>2020-07-01</v>
+      </c>
+      <c r="F3">
+        <v>79.780275792913102</v>
+      </c>
+      <c r="G3">
+        <v>77.027680998433993</v>
+      </c>
+      <c r="H3">
+        <v>82.27296593946069</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>38047</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="E4" t="str">
+        <v>2020-08-01</v>
+      </c>
+      <c r="F4">
+        <v>65.170288464675167</v>
+      </c>
+      <c r="G4">
+        <v>59.065932750368013</v>
+      </c>
+      <c r="H4">
+        <v>76.853238431257438</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>38078</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
+      </c>
+      <c r="E5" t="str">
+        <v>2020-09-01</v>
+      </c>
+      <c r="F5">
+        <v>44.016571702928744</v>
+      </c>
+      <c r="G5">
+        <v>39.733181655003428</v>
+      </c>
+      <c r="H5">
+        <v>48.644758155350424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>38108</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="E6" t="str">
+        <v>2020-10-01</v>
+      </c>
+      <c r="F6">
+        <v>38.026261891729085</v>
+      </c>
+      <c r="G6">
+        <v>34.409575807199197</v>
+      </c>
+      <c r="H6">
+        <v>40.868637330868054</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>38139</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="E7" t="str">
+        <v>2020-11-01</v>
+      </c>
+      <c r="F7">
+        <v>35.900648243933063</v>
+      </c>
+      <c r="G7">
+        <v>32.071752445354441</v>
+      </c>
+      <c r="H7">
+        <v>39.25473337419357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>38169</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="E8" t="str">
+        <v>2020-12-01</v>
+      </c>
+      <c r="F8">
+        <v>44.57935229020881</v>
+      </c>
+      <c r="G8">
+        <v>41.018106696208527</v>
+      </c>
+      <c r="H8">
+        <v>49.618038577640753</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>38200</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>38231</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>38261</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="E11" t="str" cm="1">
+        <f t="array" ref="E11:H17">_xldudf_TECHTO_FORECAST($A$1:$C$99,"Ridge",5,20,,,6,FALSE,"heater")</f>
+        <v>date</v>
+      </c>
+      <c r="F11" t="str">
+        <v>mean</v>
+      </c>
+      <c r="G11" t="str">
+        <v>lower</v>
+      </c>
+      <c r="H11" t="str">
+        <v>upper</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>38292</v>
+      </c>
+      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="E12" t="str">
+        <v>2012-03-01</v>
+      </c>
+      <c r="F12">
+        <v>15.589942627335333</v>
+      </c>
+      <c r="G12">
+        <v>13.291621669263725</v>
+      </c>
+      <c r="H12">
+        <v>17.871950436646475</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>38322</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="E13" t="str">
+        <v>2012-04-01</v>
+      </c>
+      <c r="F13">
+        <v>9.0118500702492952</v>
+      </c>
+      <c r="G13">
+        <v>5.8682353595399128</v>
+      </c>
+      <c r="H13">
+        <v>11.895928830947458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>38353</v>
+      </c>
+      <c r="B14">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="E14" t="str">
+        <v>2012-05-01</v>
+      </c>
+      <c r="F14">
+        <v>13.700570111048069</v>
+      </c>
+      <c r="G14">
+        <v>11.938635382598571</v>
+      </c>
+      <c r="H14">
+        <v>14.839434540740502</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>38384</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="E15" t="str">
+        <v>2012-06-01</v>
+      </c>
+      <c r="F15">
+        <v>8.24473712554604</v>
+      </c>
+      <c r="G15">
+        <v>6.2231070129737427</v>
+      </c>
+      <c r="H15">
+        <v>11.099130787806628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>38412</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>17</v>
+      </c>
+      <c r="E16" t="str">
+        <v>2012-07-01</v>
+      </c>
+      <c r="F16">
+        <v>9.8869076196077952</v>
+      </c>
+      <c r="G16">
+        <v>7.6994438664329312</v>
+      </c>
+      <c r="H16">
+        <v>11.88628949829474</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>38443</v>
+      </c>
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+      <c r="E17" t="str">
+        <v>2012-08-01</v>
+      </c>
+      <c r="F17">
+        <v>15.042170730936348</v>
+      </c>
+      <c r="G17">
+        <v>12.690702837626766</v>
+      </c>
+      <c r="H17">
+        <v>16.947958385017827</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>38473</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>38504</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>38534</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>29</v>
+      </c>
+      <c r="E20" t="str" cm="1">
+        <f t="array" ref="E20:O26">_xldudf_TECHTO_FORECAST($A$1:$C$99,"Ridge",5,20,,,6,TRUE,"icecream")</f>
+        <v>date</v>
+      </c>
+      <c r="F20" t="str">
+        <v>sim_1_icecream</v>
+      </c>
+      <c r="G20" t="str">
+        <v>sim_2_icecream</v>
+      </c>
+      <c r="H20" t="str">
+        <v>sim_3_icecream</v>
+      </c>
+      <c r="I20" t="str">
+        <v>sim_4_icecream</v>
+      </c>
+      <c r="J20" t="str">
+        <v>sim_5_icecream</v>
+      </c>
+      <c r="K20" t="str">
+        <v>sim_6_icecream</v>
+      </c>
+      <c r="L20" t="str">
+        <v>sim_7_icecream</v>
+      </c>
+      <c r="M20" t="str">
+        <v>sim_8_icecream</v>
+      </c>
+      <c r="N20" t="str">
+        <v>sim_9_icecream</v>
+      </c>
+      <c r="O20" t="str">
+        <v>sim_10_icecream</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>38565</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="E21" t="str">
+        <v>2012-03-01</v>
+      </c>
+      <c r="F21">
+        <v>36.729147805140194</v>
+      </c>
+      <c r="G21">
+        <v>37.650489494834439</v>
+      </c>
+      <c r="H21">
+        <v>38.968271565535446</v>
+      </c>
+      <c r="I21">
+        <v>39.468972419625914</v>
+      </c>
+      <c r="J21">
+        <v>37.505480701802526</v>
+      </c>
+      <c r="K21">
+        <v>37.920829157796938</v>
+      </c>
+      <c r="L21">
+        <v>38.521564241760331</v>
+      </c>
+      <c r="M21">
+        <v>40.283717718394549</v>
+      </c>
+      <c r="N21">
+        <v>37.136612527355751</v>
+      </c>
+      <c r="O21">
+        <v>37.31069667678409</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>38596</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>16</v>
+      </c>
+      <c r="E22" t="str">
+        <v>2012-04-01</v>
+      </c>
+      <c r="F22">
+        <v>36.468994234163169</v>
+      </c>
+      <c r="G22">
+        <v>39.008786383489046</v>
+      </c>
+      <c r="H22">
+        <v>39.205319922810745</v>
+      </c>
+      <c r="I22">
+        <v>38.197627250444739</v>
+      </c>
+      <c r="J22">
+        <v>38.129726112371969</v>
+      </c>
+      <c r="K22">
+        <v>43.671238734777248</v>
+      </c>
+      <c r="L22">
+        <v>38.823641748381895</v>
+      </c>
+      <c r="M22">
+        <v>40.226595479769102</v>
+      </c>
+      <c r="N22">
+        <v>41.471761176602925</v>
+      </c>
+      <c r="O22">
+        <v>39.85274557668351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>38626</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>14</v>
+      </c>
+      <c r="E23" t="str">
+        <v>2012-05-01</v>
+      </c>
+      <c r="F23">
+        <v>44.309052743819002</v>
+      </c>
+      <c r="G23">
+        <v>43.056681564225457</v>
+      </c>
+      <c r="H23">
+        <v>42.574852933708385</v>
+      </c>
+      <c r="I23">
+        <v>42.973414100566089</v>
+      </c>
+      <c r="J23">
+        <v>47.241540633520216</v>
+      </c>
+      <c r="K23">
+        <v>41.628261166893672</v>
+      </c>
+      <c r="L23">
+        <v>45.096422487809768</v>
+      </c>
+      <c r="M23">
+        <v>44.059192138070067</v>
+      </c>
+      <c r="N23">
+        <v>40.10511360881322</v>
+      </c>
+      <c r="O23">
+        <v>43.127799846963953</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>38657</v>
+      </c>
+      <c r="B24">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+      <c r="E24" t="str">
+        <v>2012-06-01</v>
+      </c>
+      <c r="F24">
+        <v>47.401604218901078</v>
+      </c>
+      <c r="G24">
+        <v>48.479693100360279</v>
+      </c>
+      <c r="H24">
+        <v>48.219632270377829</v>
+      </c>
+      <c r="I24">
+        <v>48.762816025037104</v>
+      </c>
+      <c r="J24">
+        <v>45.984736488039793</v>
+      </c>
+      <c r="K24">
+        <v>46.112924611680633</v>
+      </c>
+      <c r="L24">
+        <v>47.853773226293654</v>
+      </c>
+      <c r="M24">
+        <v>47.673731251663312</v>
+      </c>
+      <c r="N24">
+        <v>46.031329044763915</v>
+      </c>
+      <c r="O24">
+        <v>49.446420710503219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>38687</v>
+      </c>
+      <c r="B25">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>14</v>
+      </c>
+      <c r="E25" t="str">
+        <v>2012-07-01</v>
+      </c>
+      <c r="F25">
+        <v>46.932620812226489</v>
+      </c>
+      <c r="G25">
+        <v>47.577036628605157</v>
+      </c>
+      <c r="H25">
+        <v>46.463889085663432</v>
+      </c>
+      <c r="I25">
+        <v>48.25051851634921</v>
+      </c>
+      <c r="J25">
+        <v>46.791445640289787</v>
+      </c>
+      <c r="K25">
+        <v>49.37481979588361</v>
+      </c>
+      <c r="L25">
+        <v>46.931272972193689</v>
+      </c>
+      <c r="M25">
+        <v>45.169647710895966</v>
+      </c>
+      <c r="N25">
+        <v>46.932839157312017</v>
+      </c>
+      <c r="O25">
+        <v>48.065396459541105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>38718</v>
+      </c>
+      <c r="B26">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>14</v>
+      </c>
+      <c r="E26" t="str">
+        <v>2012-08-01</v>
+      </c>
+      <c r="F26">
+        <v>46.965436977949885</v>
+      </c>
+      <c r="G26">
+        <v>45.437136301424779</v>
+      </c>
+      <c r="H26">
+        <v>45.507531824229829</v>
+      </c>
+      <c r="I26">
+        <v>43.002697849839997</v>
+      </c>
+      <c r="J26">
+        <v>43.681645712771783</v>
+      </c>
+      <c r="K26">
+        <v>45.109587512236438</v>
+      </c>
+      <c r="L26">
+        <v>46.192701864438611</v>
+      </c>
+      <c r="M26">
+        <v>45.285025679777689</v>
+      </c>
+      <c r="N26">
+        <v>43.087906729387683</v>
+      </c>
+      <c r="O26">
+        <v>46.676614361692593</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>38749</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>38777</v>
+      </c>
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>38808</v>
+      </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>19</v>
+      </c>
+      <c r="E29" t="str" cm="1">
+        <f t="array" ref="E29:O35">_xldudf_TECHTO_FORECAST($A$1:$C$73,"Ridge",5,20,,,6,TRUE,"heater")</f>
+        <v>date</v>
+      </c>
+      <c r="F29" t="str">
+        <v>sim_1_heater</v>
+      </c>
+      <c r="G29" t="str">
+        <v>sim_2_heater</v>
+      </c>
+      <c r="H29" t="str">
+        <v>sim_3_heater</v>
+      </c>
+      <c r="I29" t="str">
+        <v>sim_4_heater</v>
+      </c>
+      <c r="J29" t="str">
+        <v>sim_5_heater</v>
+      </c>
+      <c r="K29" t="str">
+        <v>sim_6_heater</v>
+      </c>
+      <c r="L29" t="str">
+        <v>sim_7_heater</v>
+      </c>
+      <c r="M29" t="str">
+        <v>sim_8_heater</v>
+      </c>
+      <c r="N29" t="str">
+        <v>sim_9_heater</v>
+      </c>
+      <c r="O29" t="str">
+        <v>sim_10_heater</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>38838</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>23</v>
+      </c>
+      <c r="E30" t="str">
+        <v>2010-01-01</v>
+      </c>
+      <c r="F30">
+        <v>23.218928610955984</v>
+      </c>
+      <c r="G30">
+        <v>26.085141788963167</v>
+      </c>
+      <c r="H30">
+        <v>27.649505865380647</v>
+      </c>
+      <c r="I30">
+        <v>27.261431355759676</v>
+      </c>
+      <c r="J30">
+        <v>24.259011907017335</v>
+      </c>
+      <c r="K30">
+        <v>23.632521226710217</v>
+      </c>
+      <c r="L30">
+        <v>28.39893155569068</v>
+      </c>
+      <c r="M30">
+        <v>27.857147153929056</v>
+      </c>
+      <c r="N30">
+        <v>27.57978835004986</v>
+      </c>
+      <c r="O30">
+        <v>25.815847085520783</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>38869</v>
+      </c>
+      <c r="B31">
+        <v>13</v>
+      </c>
+      <c r="C31">
+        <v>27</v>
+      </c>
+      <c r="E31" t="str">
+        <v>2010-02-01</v>
+      </c>
+      <c r="F31">
+        <v>25.645124998665302</v>
+      </c>
+      <c r="G31">
+        <v>23.796145131206973</v>
+      </c>
+      <c r="H31">
+        <v>23.42911922676786</v>
+      </c>
+      <c r="I31">
+        <v>24.085379874005092</v>
+      </c>
+      <c r="J31">
+        <v>22.776454096219545</v>
+      </c>
+      <c r="K31">
+        <v>24.204562682677224</v>
+      </c>
+      <c r="L31">
+        <v>24.664815890226755</v>
+      </c>
+      <c r="M31">
+        <v>23.836204471347877</v>
+      </c>
+      <c r="N31">
+        <v>23.933968509828919</v>
+      </c>
+      <c r="O31">
+        <v>24.331035757640141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>38899</v>
+      </c>
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <v>32</v>
+      </c>
+      <c r="E32" t="str">
+        <v>2010-03-01</v>
+      </c>
+      <c r="F32">
+        <v>19.797748008956734</v>
+      </c>
+      <c r="G32">
+        <v>18.481677430321582</v>
+      </c>
+      <c r="H32">
+        <v>17.122004192718499</v>
+      </c>
+      <c r="I32">
+        <v>20.135344224630774</v>
+      </c>
+      <c r="J32">
+        <v>20.048449658816324</v>
+      </c>
+      <c r="K32">
+        <v>17.902909425735814</v>
+      </c>
+      <c r="L32">
+        <v>19.064604068817911</v>
+      </c>
+      <c r="M32">
+        <v>18.128445855852767</v>
+      </c>
+      <c r="N32">
+        <v>18.677000338732405</v>
+      </c>
+      <c r="O32">
+        <v>17.704458369760754</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>38930</v>
+      </c>
+      <c r="B33">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>24</v>
+      </c>
+      <c r="E33" t="str">
+        <v>2010-04-01</v>
+      </c>
+      <c r="F33">
+        <v>14.124690859226684</v>
+      </c>
+      <c r="G33">
+        <v>12.221350267584098</v>
+      </c>
+      <c r="H33">
+        <v>14.444379882054148</v>
+      </c>
+      <c r="I33">
+        <v>14.272986221930251</v>
+      </c>
+      <c r="J33">
+        <v>14.656637862897885</v>
+      </c>
+      <c r="K33">
+        <v>15.481614800295022</v>
+      </c>
+      <c r="L33">
+        <v>14.394410792094789</v>
+      </c>
+      <c r="M33">
+        <v>13.883967580611063</v>
+      </c>
+      <c r="N33">
+        <v>14.110550154654137</v>
+      </c>
+      <c r="O33">
+        <v>15.135361658346309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>38961</v>
+      </c>
+      <c r="B34">
+        <v>16</v>
+      </c>
+      <c r="C34">
+        <v>19</v>
+      </c>
+      <c r="E34" t="str">
+        <v>2010-05-01</v>
+      </c>
+      <c r="F34">
+        <v>12.05493720860461</v>
+      </c>
+      <c r="G34">
+        <v>11.505068503746422</v>
+      </c>
+      <c r="H34">
+        <v>14.462502929146918</v>
+      </c>
+      <c r="I34">
+        <v>15.08598284798407</v>
+      </c>
+      <c r="J34">
+        <v>12.418195139671344</v>
+      </c>
+      <c r="K34">
+        <v>14.039798839414621</v>
+      </c>
+      <c r="L34">
+        <v>14.32195047858059</v>
+      </c>
+      <c r="M34">
+        <v>14.011819277380514</v>
+      </c>
+      <c r="N34">
+        <v>12.567433372287264</v>
+      </c>
+      <c r="O34">
+        <v>14.341557438249774</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>38991</v>
+      </c>
+      <c r="B35">
+        <v>22</v>
+      </c>
+      <c r="C35">
+        <v>16</v>
+      </c>
+      <c r="E35" t="str">
+        <v>2010-06-01</v>
+      </c>
+      <c r="F35">
+        <v>12.314007896342597</v>
+      </c>
+      <c r="G35">
+        <v>14.094028205742408</v>
+      </c>
+      <c r="H35">
+        <v>12.519621148068298</v>
+      </c>
+      <c r="I35">
+        <v>12.744142997483571</v>
+      </c>
+      <c r="J35">
+        <v>12.692090258905822</v>
+      </c>
+      <c r="K35">
+        <v>12.394247129483389</v>
+      </c>
+      <c r="L35">
+        <v>13.889948850608006</v>
+      </c>
+      <c r="M35">
+        <v>15.477588330347723</v>
+      </c>
+      <c r="N35">
+        <v>14.194306113853264</v>
+      </c>
+      <c r="O35">
+        <v>13.567764897794614</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>39022</v>
+      </c>
+      <c r="B36">
+        <v>23</v>
+      </c>
+      <c r="C36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>39052</v>
+      </c>
+      <c r="B37">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>39083</v>
+      </c>
+      <c r="B38">
+        <v>25</v>
+      </c>
+      <c r="C38">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>39114</v>
+      </c>
+      <c r="B39">
+        <v>23</v>
+      </c>
+      <c r="C39">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39142</v>
+      </c>
+      <c r="B40">
+        <v>16</v>
+      </c>
+      <c r="C40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>39173</v>
+      </c>
+      <c r="B41">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>39203</v>
+      </c>
+      <c r="B42">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>39234</v>
+      </c>
+      <c r="B43">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>39264</v>
+      </c>
+      <c r="B44">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>39295</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>39326</v>
+      </c>
+      <c r="B46">
+        <v>15</v>
+      </c>
+      <c r="C46">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>39356</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>39387</v>
+      </c>
+      <c r="B48">
+        <v>26</v>
+      </c>
+      <c r="C48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>39417</v>
+      </c>
+      <c r="B49">
+        <v>29</v>
+      </c>
+      <c r="C49">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>39448</v>
+      </c>
+      <c r="B50">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>39479</v>
+      </c>
+      <c r="B51">
+        <v>20</v>
+      </c>
+      <c r="C51">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>39508</v>
+      </c>
+      <c r="B52">
+        <v>16</v>
+      </c>
+      <c r="C52">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>39539</v>
+      </c>
+      <c r="B53">
+        <v>15</v>
+      </c>
+      <c r="C53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>39569</v>
+      </c>
+      <c r="B54">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>39600</v>
+      </c>
+      <c r="B55">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>39630</v>
+      </c>
+      <c r="B56">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>39661</v>
+      </c>
+      <c r="B57">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>39692</v>
+      </c>
+      <c r="B58">
+        <v>17</v>
+      </c>
+      <c r="C58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>39722</v>
+      </c>
+      <c r="B59">
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>39753</v>
+      </c>
+      <c r="B60">
+        <v>28</v>
+      </c>
+      <c r="C60">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>39783</v>
+      </c>
+      <c r="B61">
+        <v>31</v>
+      </c>
+      <c r="C61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>39814</v>
+      </c>
+      <c r="B62">
+        <v>29</v>
+      </c>
+      <c r="C62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>39845</v>
+      </c>
+      <c r="B63">
+        <v>21</v>
+      </c>
+      <c r="C63">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>39873</v>
+      </c>
+      <c r="B64">
+        <v>17</v>
+      </c>
+      <c r="C64">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>39904</v>
+      </c>
+      <c r="B65">
+        <v>15</v>
+      </c>
+      <c r="C65">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>39934</v>
+      </c>
+      <c r="B66">
+        <v>14</v>
+      </c>
+      <c r="C66">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>39965</v>
+      </c>
+      <c r="B67">
+        <v>14</v>
+      </c>
+      <c r="C67">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>39995</v>
+      </c>
+      <c r="B68">
+        <v>13</v>
+      </c>
+      <c r="C68">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>40026</v>
+      </c>
+      <c r="B69">
+        <v>13</v>
+      </c>
+      <c r="C69">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>40057</v>
+      </c>
+      <c r="B70">
+        <v>16</v>
+      </c>
+      <c r="C70">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>40087</v>
+      </c>
+      <c r="B71">
+        <v>24</v>
+      </c>
+      <c r="C71">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>40118</v>
+      </c>
+      <c r="B72">
+        <v>23</v>
+      </c>
+      <c r="C72">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>40148</v>
+      </c>
+      <c r="B73">
+        <v>33</v>
+      </c>
+      <c r="C73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>40179</v>
+      </c>
+      <c r="B74">
+        <v>30</v>
+      </c>
+      <c r="C74">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>40210</v>
+      </c>
+      <c r="B75">
+        <v>22</v>
+      </c>
+      <c r="C75">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>40238</v>
+      </c>
+      <c r="B76">
+        <v>17</v>
+      </c>
+      <c r="C76">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>40269</v>
+      </c>
+      <c r="B77">
+        <v>15</v>
+      </c>
+      <c r="C77">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>40299</v>
+      </c>
+      <c r="B78">
+        <v>14</v>
+      </c>
+      <c r="C78">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>40330</v>
+      </c>
+      <c r="B79">
+        <v>12</v>
+      </c>
+      <c r="C79">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>40360</v>
+      </c>
+      <c r="B80">
+        <v>11</v>
+      </c>
+      <c r="C80">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>40391</v>
+      </c>
+      <c r="B81">
+        <v>12</v>
+      </c>
+      <c r="C81">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>40422</v>
+      </c>
+      <c r="B82">
+        <v>14</v>
+      </c>
+      <c r="C82">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>40452</v>
+      </c>
+      <c r="B83">
+        <v>21</v>
+      </c>
+      <c r="C83">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>40483</v>
+      </c>
+      <c r="B84">
+        <v>27</v>
+      </c>
+      <c r="C84">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>40513</v>
+      </c>
+      <c r="B85">
+        <v>32</v>
+      </c>
+      <c r="C85">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>40544</v>
+      </c>
+      <c r="B86">
+        <v>31</v>
+      </c>
+      <c r="C86">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>40575</v>
+      </c>
+      <c r="B87">
+        <v>24</v>
+      </c>
+      <c r="C87">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>40603</v>
+      </c>
+      <c r="B88">
+        <v>18</v>
+      </c>
+      <c r="C88">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>40634</v>
+      </c>
+      <c r="B89">
+        <v>15</v>
+      </c>
+      <c r="C89">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>40664</v>
+      </c>
+      <c r="B90">
+        <v>14</v>
+      </c>
+      <c r="C90">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>40695</v>
+      </c>
+      <c r="B91">
+        <v>14</v>
+      </c>
+      <c r="C91">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>40725</v>
+      </c>
+      <c r="B92">
+        <v>13</v>
+      </c>
+      <c r="C92">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>40756</v>
+      </c>
+      <c r="B93">
+        <v>14</v>
+      </c>
+      <c r="C93">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>40787</v>
+      </c>
+      <c r="B94">
+        <v>17</v>
+      </c>
+      <c r="C94">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>40817</v>
+      </c>
+      <c r="B95">
+        <v>25</v>
+      </c>
+      <c r="C95">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>40848</v>
+      </c>
+      <c r="B96">
+        <v>31</v>
+      </c>
+      <c r="C96">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>40878</v>
+      </c>
+      <c r="B97">
+        <v>32</v>
+      </c>
+      <c r="C97">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>40909</v>
+      </c>
+      <c r="B98">
+        <v>28</v>
+      </c>
+      <c r="C98">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>40940</v>
+      </c>
+      <c r="B99">
+        <v>21</v>
+      </c>
+      <c r="C99">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>40969</v>
+      </c>
+      <c r="B100">
+        <v>17</v>
+      </c>
+      <c r="C100">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>41000</v>
+      </c>
+      <c r="B101">
+        <v>15</v>
+      </c>
+      <c r="C101">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>41030</v>
+      </c>
+      <c r="B102">
+        <v>14</v>
+      </c>
+      <c r="C102">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>41061</v>
+      </c>
+      <c r="B103">
+        <v>13</v>
+      </c>
+      <c r="C103">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>41091</v>
+      </c>
+      <c r="B104">
+        <v>13</v>
+      </c>
+      <c r="C104">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>41122</v>
+      </c>
+      <c r="B105">
+        <v>13</v>
+      </c>
+      <c r="C105">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>41153</v>
+      </c>
+      <c r="B106">
+        <v>16</v>
+      </c>
+      <c r="C106">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>41183</v>
+      </c>
+      <c r="B107">
+        <v>25</v>
+      </c>
+      <c r="C107">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>41214</v>
+      </c>
+      <c r="B108">
+        <v>32</v>
+      </c>
+      <c r="C108">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>41244</v>
+      </c>
+      <c r="B109">
+        <v>29</v>
+      </c>
+      <c r="C109">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>41275</v>
+      </c>
+      <c r="B110">
+        <v>30</v>
+      </c>
+      <c r="C110">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>41306</v>
+      </c>
+      <c r="B111">
+        <v>23</v>
+      </c>
+      <c r="C111">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>41334</v>
+      </c>
+      <c r="B112">
+        <v>20</v>
+      </c>
+      <c r="C112">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>41365</v>
+      </c>
+      <c r="B113">
+        <v>16</v>
+      </c>
+      <c r="C113">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>41395</v>
+      </c>
+      <c r="B114">
+        <v>15</v>
+      </c>
+      <c r="C114">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>41426</v>
+      </c>
+      <c r="B115">
+        <v>14</v>
+      </c>
+      <c r="C115">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>41456</v>
+      </c>
+      <c r="B116">
+        <v>14</v>
+      </c>
+      <c r="C116">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>41487</v>
+      </c>
+      <c r="B117">
+        <v>14</v>
+      </c>
+      <c r="C117">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>41518</v>
+      </c>
+      <c r="B118">
+        <v>17</v>
+      </c>
+      <c r="C118">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>41548</v>
+      </c>
+      <c r="B119">
+        <v>27</v>
+      </c>
+      <c r="C119">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>41579</v>
+      </c>
+      <c r="B120">
+        <v>36</v>
+      </c>
+      <c r="C120">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>41609</v>
+      </c>
+      <c r="B121">
+        <v>39</v>
+      </c>
+      <c r="C121">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>41640</v>
+      </c>
+      <c r="B122">
+        <v>39</v>
+      </c>
+      <c r="C122">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>41671</v>
+      </c>
+      <c r="B123">
+        <v>28</v>
+      </c>
+      <c r="C123">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>41699</v>
+      </c>
+      <c r="B124">
+        <v>21</v>
+      </c>
+      <c r="C124">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>41730</v>
+      </c>
+      <c r="B125">
+        <v>17</v>
+      </c>
+      <c r="C125">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>41760</v>
+      </c>
+      <c r="B126">
+        <v>16</v>
+      </c>
+      <c r="C126">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>41791</v>
+      </c>
+      <c r="B127">
+        <v>15</v>
+      </c>
+      <c r="C127">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>41821</v>
+      </c>
+      <c r="B128">
+        <v>15</v>
+      </c>
+      <c r="C128">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>41852</v>
+      </c>
+      <c r="B129">
+        <v>16</v>
+      </c>
+      <c r="C129">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>41883</v>
+      </c>
+      <c r="B130">
+        <v>19</v>
+      </c>
+      <c r="C130">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>41913</v>
+      </c>
+      <c r="B131">
+        <v>26</v>
+      </c>
+      <c r="C131">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>41944</v>
+      </c>
+      <c r="B132">
+        <v>45</v>
+      </c>
+      <c r="C132">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>41974</v>
+      </c>
+      <c r="B133">
+        <v>32</v>
+      </c>
+      <c r="C133">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>42005</v>
+      </c>
+      <c r="B134">
+        <v>36</v>
+      </c>
+      <c r="C134">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B135">
+        <v>32</v>
+      </c>
+      <c r="C135">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>42064</v>
+      </c>
+      <c r="B136">
+        <v>21</v>
+      </c>
+      <c r="C136">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>42095</v>
+      </c>
+      <c r="B137">
+        <v>17</v>
+      </c>
+      <c r="C137">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>42125</v>
+      </c>
+      <c r="B138">
+        <v>17</v>
+      </c>
+      <c r="C138">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>42156</v>
+      </c>
+      <c r="B139">
+        <v>17</v>
+      </c>
+      <c r="C139">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>42186</v>
+      </c>
+      <c r="B140">
+        <v>16</v>
+      </c>
+      <c r="C140">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>42217</v>
+      </c>
+      <c r="B141">
+        <v>17</v>
+      </c>
+      <c r="C141">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>42248</v>
+      </c>
+      <c r="B142">
+        <v>19</v>
+      </c>
+      <c r="C142">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>42278</v>
+      </c>
+      <c r="B143">
+        <v>29</v>
+      </c>
+      <c r="C143">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>42309</v>
+      </c>
+      <c r="B144">
+        <v>37</v>
+      </c>
+      <c r="C144">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>42339</v>
+      </c>
+      <c r="B145">
+        <v>35</v>
+      </c>
+      <c r="C145">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>42370</v>
+      </c>
+      <c r="B146">
+        <v>40</v>
+      </c>
+      <c r="C146">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>42401</v>
+      </c>
+      <c r="B147">
+        <v>28</v>
+      </c>
+      <c r="C147">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>42430</v>
+      </c>
+      <c r="B148">
+        <v>21</v>
+      </c>
+      <c r="C148">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>42461</v>
+      </c>
+      <c r="B149">
+        <v>20</v>
+      </c>
+      <c r="C149">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>42491</v>
+      </c>
+      <c r="B150">
+        <v>19</v>
+      </c>
+      <c r="C150">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>42522</v>
+      </c>
+      <c r="B151">
+        <v>18</v>
+      </c>
+      <c r="C151">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B152">
+        <v>17</v>
+      </c>
+      <c r="C152">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>42583</v>
+      </c>
+      <c r="B153">
+        <v>17</v>
+      </c>
+      <c r="C153">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B154">
+        <v>21</v>
+      </c>
+      <c r="C154">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>42644</v>
+      </c>
+      <c r="B155">
+        <v>29</v>
+      </c>
+      <c r="C155">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>42675</v>
+      </c>
+      <c r="B156">
+        <v>39</v>
+      </c>
+      <c r="C156">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>42705</v>
+      </c>
+      <c r="B157">
+        <v>52</v>
+      </c>
+      <c r="C157">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>42736</v>
+      </c>
+      <c r="B158">
+        <v>40</v>
+      </c>
+      <c r="C158">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>42767</v>
+      </c>
+      <c r="B159">
+        <v>27</v>
+      </c>
+      <c r="C159">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>42795</v>
+      </c>
+      <c r="B160">
+        <v>25</v>
+      </c>
+      <c r="C160">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>42826</v>
+      </c>
+      <c r="B161">
+        <v>20</v>
+      </c>
+      <c r="C161">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>42856</v>
+      </c>
+      <c r="B162">
+        <v>21</v>
+      </c>
+      <c r="C162">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>42887</v>
+      </c>
+      <c r="B163">
+        <v>20</v>
+      </c>
+      <c r="C163">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>42917</v>
+      </c>
+      <c r="B164">
+        <v>19</v>
+      </c>
+      <c r="C164">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>42948</v>
+      </c>
+      <c r="B165">
+        <v>19</v>
+      </c>
+      <c r="C165">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>42979</v>
+      </c>
+      <c r="B166">
+        <v>23</v>
+      </c>
+      <c r="C166">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>43009</v>
+      </c>
+      <c r="B167">
+        <v>33</v>
+      </c>
+      <c r="C167">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>43040</v>
+      </c>
+      <c r="B168">
+        <v>43</v>
+      </c>
+      <c r="C168">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>43070</v>
+      </c>
+      <c r="B169">
+        <v>56</v>
+      </c>
+      <c r="C169">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B170">
+        <v>56</v>
+      </c>
+      <c r="C170">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B171">
+        <v>33</v>
+      </c>
+      <c r="C171">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>43160</v>
+      </c>
+      <c r="B172">
+        <v>27</v>
+      </c>
+      <c r="C172">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>43191</v>
+      </c>
+      <c r="B173">
+        <v>24</v>
+      </c>
+      <c r="C173">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B174">
+        <v>22</v>
+      </c>
+      <c r="C174">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>43252</v>
+      </c>
+      <c r="B175">
+        <v>21</v>
+      </c>
+      <c r="C175">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B176">
+        <v>21</v>
+      </c>
+      <c r="C176">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>43313</v>
+      </c>
+      <c r="B177">
+        <v>21</v>
+      </c>
+      <c r="C177">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B178">
+        <v>24</v>
+      </c>
+      <c r="C178">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B179">
+        <v>39</v>
+      </c>
+      <c r="C179">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B180">
+        <v>53</v>
+      </c>
+      <c r="C180">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>43435</v>
+      </c>
+      <c r="B181">
+        <v>48</v>
+      </c>
+      <c r="C181">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B182">
+        <v>49</v>
+      </c>
+      <c r="C182">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>43497</v>
+      </c>
+      <c r="B183">
+        <v>39</v>
+      </c>
+      <c r="C183">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>43525</v>
+      </c>
+      <c r="B184">
+        <v>30</v>
+      </c>
+      <c r="C184">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>43556</v>
+      </c>
+      <c r="B185">
+        <v>24</v>
+      </c>
+      <c r="C185">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>43586</v>
+      </c>
+      <c r="B186">
+        <v>23</v>
+      </c>
+      <c r="C186">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B187">
+        <v>22</v>
+      </c>
+      <c r="C187">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>43647</v>
+      </c>
+      <c r="B188">
+        <v>21</v>
+      </c>
+      <c r="C188">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>43678</v>
+      </c>
+      <c r="B189">
+        <v>21</v>
+      </c>
+      <c r="C189">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>43709</v>
+      </c>
+      <c r="B190">
+        <v>24</v>
+      </c>
+      <c r="C190">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>43739</v>
+      </c>
+      <c r="B191">
+        <v>40</v>
+      </c>
+      <c r="C191">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>43770</v>
+      </c>
+      <c r="B192">
+        <v>56</v>
+      </c>
+      <c r="C192">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B193">
+        <v>46</v>
+      </c>
+      <c r="C193">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B194">
+        <v>41</v>
+      </c>
+      <c r="C194">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B195">
+        <v>34</v>
+      </c>
+      <c r="C195">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B196">
+        <v>25</v>
+      </c>
+      <c r="C196">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B197">
+        <v>25</v>
+      </c>
+      <c r="C197">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B198">
+        <v>27</v>
+      </c>
+      <c r="C198">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B199">
+        <v>24</v>
+      </c>
+      <c r="C199">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
do multivariate case Pt.4
</commit_message>
<xml_diff>
--- a/examples/excel_formulas.xlsx
+++ b/examples/excel_formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t/Documents/Python_Packages/techtonique-apis/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D9ADDC-DE17-C94E-802A-EA71472F2942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1CB1A6-4EA6-674B-9EBF-ED49AAAFCDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14720" activeTab="1" xr2:uid="{866FC63A-F4EA-0B48-8E6B-E2860E222B05}"/>
   </bookViews>
@@ -672,10 +672,10 @@
     <we:reference id="wa200008175" version="1.0.0.0" store="en-US" storeType="OMEX"/>
   </we:alternateReferences>
   <we:properties>
-    <we:property name="main.py" value="&quot;\&quot;\&quot;\&quot;\nxlwings Lite allows you to define\nautomation scripts and custom functions\nwith Python instead of VBA\/Office Scripts.\n\nSelect a function in the green dropdown\nabove and run it by clicking the button or\nor by pressing F5. One of the sample\nscripts will insert custom functions,\nwhich are defined using the @func\ndecorator. You can add, delete, or edit\nfunctions in this file.\&quot;\&quot;\&quot;\nimport tempfile\nimport datetime as dt\nimport numpy as np\nimport pandas as pd\nimport seaborn as sns\nfrom xlwings import func, arg, ret\nfrom techtonique_apis import TechtoniqueAPI\n\n@func\ndef hello(name: str):\n    # This is the easiest custom function\n    return f\&quot;Hello {name}!\&quot;\n\n\n@func\ndef standard_normal(rows, cols):\n    # Returns an array of standard normally distributed pseudo random numbers\n    rng = np.random.default_rng()\n    matrix = rng.standard_normal(size=(rows, cols))\n    date_rng = pd.date_range(start=dt.datetime(2025, 6, 15), periods=rows, freq=\&quot;D\&quot;)\n    df = pd.DataFrame(\n        matrix, columns=[f\&quot;col{i + 1}\&quot; for i in range(matrix.shape[1])], index=date_rng\n    )\n    return df\n\n\n@func\ndef correl2(df: pd.DataFrame):\n    # Like CORREL, but it works on whole matrices instead of just 2 arrays.\n    # The type hint converts the values of the range into a pandas DataFrame.\n    # Use this function on the output of the standard_normal function from above.\n    return df.corr()\n\napi = TechtoniqueAPI()\n\ndef excel_date_to_datetime(excel_serial):\n    # Excel's day 0 is 1899-12-30\n    return pd.to_datetime('1899-12-30') + pd.to_timedelta(excel_serial, unit='D')\n\n@func\n@arg(\&quot;df\&quot;, index=False)\n@ret(index=False)\ndef techto_forecast(\n    df: pd.DataFrame,\n    base_model: str = \&quot;RidgeCV\&quot;,\n    n_hidden_features: int = 5,\n    lags: int = 25,\n    type_pi: str = \&quot;kde\&quot;,\n    replications: int = 10,\n    h: int = 5,\n    return_sims: bool = False, \n    series_choice: str = None\n) -&gt; pd.DataFrame:\n    \&quot;\&quot;\&quot;Forecasting: pass a time series as a DataFrame from Excel, return forecast.\n    \n    Excel\/xlwings custom function: Forecast a time series passed as a DataFrame from Excel, using the Techtonique API.\n\n    Parameters\n    ----------\n\n    df : pd.DataFrame\n        The input time series data as a DataFrame (from Excel range).\n\n    base_model : str, default \&quot;RidgeCV\&quot;\n        The base model to use for forecasting.\n\n    n_hidden_features : int, default 5\n        Number of hidden features for the model.\n\n    lags : int, default 25\n        Number of lags to use in the model.\n\n    type_pi : str, default \&quot;kde\&quot;\n        Type of prediction interval (\&quot;kde\&quot; or other supported types).\n\n    replications : int, default 10\n        Number of simulation replications.\n\n    h : int, default 5\n        Forecast horizon (number of periods ahead to forecast).\n\n    return_sims : bool, default False\n        If True, return the simulation matrix; otherwise, return the forecast summary bounds.\n    \n    series_choice : str, optional\n        If provided, specifies which series to forecast from the DataFrame.\n\n    Returns\n    -------\n\n    pd.DataFrame\n        The forecast results or simulation matrix as a DataFrame for Excel.\n\n    \&quot;\&quot;\&quot;\n    # Convert Excel serial dates to datetime if needed\n    if pd.api.types.is_numeric_dtype(df['date']):\n        df['date'] = df['date'].apply(excel_date_to_datetime)\n\n    with tempfile.NamedTemporaryFile(suffix=\&quot;.csv\&quot;, delete=False) as tmp:\n        df.to_csv(tmp.name, index=False)\n        result = api.forecasting(\n            file_path=tmp.name,\n            base_model=base_model,\n            n_hidden_features=n_hidden_features,\n            lags=lags,\n            type_pi=type_pi,\n            replications=replications,\n            h=h,\n        )\n    output_dates = result[\&quot;date\&quot;]\n    if df.shape[1] == 2: # univariate time series\n        res_df = pd.DataFrame(result.pop('sims'))\n        if return_sims:\n            res2_df = pd.DataFrame([])\n            res2_df[\&quot;date\&quot;] = output_dates\n            sims_df = res_df.transpose()\n            sims_df.columns = [(i + 1) for i in range(sims_df.shape[1])]\n            return pd.concat([res2_df, sims_df], axis=1)\n        return pd.DataFrame(result)\n    else:  # multivariate time series\n        n_series = len(result[\&quot;mean\&quot;][0])\n        series_names = [col for col in df.columns if col != \&quot;date\&quot;]\n        if len(series_names) != n_series:\n            series_names = [f\&quot;series_{i+1}\&quot; for i in range(n_series)]\n\n        # If series_choice is provided and valid, extract its index and return as univariate\n        if series_choice is not None and series_choice in series_names:\n            idx = series_names.index(series_choice)\n            # Extract only the selected series from each stat\n            summary_df = pd.DataFrame({\n                \&quot;date\&quot;: output_dates,\n                \&quot;mean\&quot;: [x[idx] for x in result[\&quot;mean\&quot;]],\n                \&quot;lower\&quot;: [x[idx] for x in result[\&quot;lower\&quot;]],\n                \&quot;upper\&quot;: [x[idx] for x in result[\&quot;upper\&quot;]],\n            })\n            if return_sims:\n                # sims: shape (replications, horizon, n_series)\n                sims = result[\&quot;sims\&quot;]  # list of replications, each is list of horizon, each is list of n_series\n                # For each replication, extract the selected series only\n                sims_selected = [[h[idx] for h in rep] for rep in sims]  # shape: (replications, horizon)\n                sims_df = pd.DataFrame(sims_selected).transpose()\n                sims_df.columns = [f\&quot;sim_{i+1}_{series_choice}\&quot; for i in range(sims_df.shape[1])]\n                res2_df = pd.DataFrame({\&quot;date\&quot;: output_dates})\n                return pd.concat([res2_df, sims_df], axis=1)\n            return summary_df\n\n        # Otherwise, return the full multivariate summary as before\n        summary_data = {\&quot;date\&quot;: output_dates}\n        for stat in [\&quot;mean\&quot;, \&quot;lower\&quot;, \&quot;upper\&quot;]:\n            for s in range(n_series):\n                summary_data[f\&quot;{stat}_{series_names[s]}\&quot;] = [x[s] for x in result[stat]]\n        summary_df = pd.DataFrame(summary_data)\n        if return_sims:\n            # sims: shape (replications, horizon, n_series)\n            sims = result[\&quot;sims\&quot;]\n            flat = []\n            for rep in sims:\n                for s in range(n_series):\n                    flat.append([h[s] for h in rep])\n            sims_df = pd.DataFrame(flat).transpose()\n            colnames = []\n            for r in range(len(sims)):\n                for s in range(n_series):\n                    colnames.append(f\&quot;sim_{r+1}_{series_names[s]}\&quot;)\n            sims_df.columns = colnames\n            sims_df.insert(0, \&quot;date\&quot;, output_dates)\n            return sims_df\n        return summary_df\n\n\n\n&quot;"/>
+    <we:property name="main.py" value="&quot;from techtonique_apis import techto_forecast&quot;"/>
     <we:property name="pyodideVersion" value="&quot;0.27.5&quot;"/>
     <we:property name="addinVersion" value="&quot;1.0.0.0-17&quot;"/>
-    <we:property name="requirements.txt" value="&quot;# Pin the version of packages that are installed from PyPI.\n# Don't pin the version if they are on this list:\n# https:\/\/pyodide.org\/en\/stable\/usage\/packages-in-pyodide.html\n#\n# New packages are installed on the fly.\n# However, the following situations require a restart:\n# - removing a package\n# - changing the version of a package\n# - adding an optional dependency of xlwings, e.g, polars\n\nxlwings==0.33.14  # required\npython-dotenv==1.1.0  # required\npyodide-http  # required\nblack  # required\npandas\nmatplotlib\nseaborn\ntechtonique_apis&quot;"/>
+    <we:property name="requirements.txt" value="&quot;xlwings==0.33.14  # required\npython-dotenv==1.1.0  # required\npyodide-http  # required\nblack  # required\ntechtonique_apis&quot;"/>
   </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
@@ -700,7 +700,7 @@
   <dimension ref="A1:X73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2078,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0DF073-385F-1248-B9C4-6F72C369E2B0}">
   <dimension ref="A1:O199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add excel docstrings Pt.2
</commit_message>
<xml_diff>
--- a/examples/excel_formulas.xlsx
+++ b/examples/excel_formulas.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/t/Documents/Python_Packages/techtonique-apis/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1CB1A6-4EA6-674B-9EBF-ED49AAAFCDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A20CCC-DBA0-E14E-92BE-A6F312C2333D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14720" activeTab="1" xr2:uid="{866FC63A-F4EA-0B48-8E6B-E2860E222B05}"/>
   </bookViews>
   <sheets>
-    <sheet name="univariate" sheetId="1" r:id="rId1"/>
-    <sheet name="multivariate" sheetId="2" r:id="rId2"/>
+    <sheet name="univariate forecasting" sheetId="1" r:id="rId1"/>
+    <sheet name="multivariate forecasting" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -700,7 +700,7 @@
   <dimension ref="A1:X73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2079,7 +2079,7 @@
   <dimension ref="A1:O199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>